<commit_message>
refresh EEIO factor w/ updated data
</commit_message>
<xml_diff>
--- a/data/RStudio Air Travel Data.xlsx
+++ b/data/RStudio Air Travel Data.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="36">
   <si>
     <t>departure_airport</t>
   </si>
@@ -23,6 +23,9 @@
     <t>roundtrip</t>
   </si>
   <si>
+    <t>layover</t>
+  </si>
+  <si>
     <t>description</t>
   </si>
   <si>
@@ -56,22 +59,49 @@
     <t>CMH</t>
   </si>
   <si>
+    <t>roundrip</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
     <t>work week</t>
   </si>
   <si>
+    <t>BOS</t>
+  </si>
+  <si>
+    <t>one way</t>
+  </si>
+  <si>
+    <t>IDS + Oasis Conferences (departure flight 1)</t>
+  </si>
+  <si>
     <t>ZRH</t>
   </si>
   <si>
-    <t>IDS + Oasis Conferences</t>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>IDS + Oasis Conferences (departure flight 2+3)</t>
+  </si>
+  <si>
+    <t>LIN</t>
+  </si>
+  <si>
+    <t>CDG</t>
+  </si>
+  <si>
+    <t>IDS + Oasis Conferences (return flight 1)</t>
+  </si>
+  <si>
+    <t>IDS + Oasis Conferences (return flight 2)</t>
   </si>
   <si>
     <t>TLS</t>
   </si>
   <si>
     <t>Toulouse useR!</t>
-  </si>
-  <si>
-    <t>BOS</t>
   </si>
   <si>
     <t>Richardson Training (direct)</t>
@@ -97,10 +127,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -112,16 +142,30 @@
       <name val="Arial"/>
     </font>
     <font>
+      <b/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8ECED"/>
+        <bgColor rgb="FFE8ECED"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -130,21 +174,34 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -367,7 +424,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="4" max="4" width="33.86"/>
+    <col customWidth="1" min="4" max="4" width="12.57"/>
+    <col customWidth="1" min="5" max="5" width="40.86"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -380,7 +438,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -395,207 +453,318 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
+      <c r="A2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="3">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="4">
         <v>2480.0</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="G2" s="4"/>
+      <c r="H2" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="I2" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="3">
+      <c r="C3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="4">
         <v>3700.0</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="G3" s="5">
+        <v>560.6</v>
+      </c>
+      <c r="H3" s="6">
+        <v>43604.0</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="5">
+        <v>5640.0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>291.3</v>
+      </c>
+      <c r="H4" s="6">
+        <v>43682.0</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="7">
+        <f>(3875+2634)</f>
+        <v>6509</v>
+      </c>
+      <c r="G5" s="5">
+        <v>822.72</v>
+      </c>
+      <c r="H5" s="6">
+        <v>43626.0</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="5">
+        <v>641.0</v>
+      </c>
+      <c r="G6" s="4">
+        <f>177/2</f>
+        <v>88.5</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="8">
+        <v>7838.0</v>
+      </c>
+      <c r="G7" s="4">
+        <f>899/2</f>
+        <v>449.5</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="4">
+        <v>17956.0</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="3">
-        <v>17640.0</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3" t="s">
+      <c r="I8" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="3">
-        <v>17956.0</v>
-      </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="C9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="4">
         <v>5640.0</v>
       </c>
-      <c r="F6" s="4">
+      <c r="G9" s="9">
         <f>259.3+147.3</f>
         <v>406.6</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="3" t="s">
+      <c r="H9" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="3">
+      <c r="I9" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="4">
         <v>5640.0</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="3" t="s">
+      <c r="G10" s="4"/>
+      <c r="H10" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="I10" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="3">
+      <c r="D11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="4">
         <v>4240.0</v>
       </c>
-      <c r="F8" s="4">
+      <c r="G11" s="9">
         <v>902.05</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="H11" s="4"/>
+      <c r="I11" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="4">
+      <c r="D12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="9">
         <v>252.6</v>
       </c>
-      <c r="G9" s="5">
+      <c r="H12" s="10">
         <v>43856.0</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>12</v>
+      <c r="I12" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>